<commit_message>
Bugfix: Lua load none e config ID will crashed!
</commit_message>
<xml_diff>
--- a/resource/excel/Scene.xlsx
+++ b/resource/excel/Scene.xlsx
@@ -4,12 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26136" windowHeight="16260"/>
+    <workbookView windowWidth="20930" windowHeight="8850"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -106,7 +119,7 @@
     <t>actorid</t>
   </si>
   <si>
-    <t>1</t>
+    <t>SceneID_1</t>
   </si>
   <si>
     <t>World</t>
@@ -121,7 +134,7 @@
     <t>10,10,10</t>
   </si>
   <si>
-    <t>2</t>
+    <t>SceneID_2</t>
   </si>
   <si>
     <t>Lobby</t>
@@ -130,7 +143,7 @@
     <t>玩家个人大厅</t>
   </si>
   <si>
-    <t>3</t>
+    <t>SceneID_3</t>
   </si>
   <si>
     <t>PvpRoom</t>
@@ -142,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -166,43 +179,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -210,62 +195,69 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -273,7 +265,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -281,14 +273,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -296,24 +288,45 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -342,49 +355,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,121 +493,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,21 +661,6 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,6 +694,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,148 +767,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -947,55 +960,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -1338,22 +1351,22 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="15.1296296296296" customWidth="1"/>
-    <col min="2" max="2" width="16.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="18.212962962963" customWidth="1"/>
-    <col min="4" max="4" width="21.4444444444444" customWidth="1"/>
-    <col min="5" max="5" width="17.1111111111111" customWidth="1"/>
-    <col min="6" max="8" width="53.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="8.87962962962963" customWidth="1"/>
-    <col min="10" max="10" width="27.3333333333333" customWidth="1"/>
-    <col min="11" max="11" width="40.75" customWidth="1"/>
-    <col min="12" max="12" width="27.3333333333333" customWidth="1"/>
-    <col min="13" max="13" width="9.33333333333333" customWidth="1"/>
+    <col min="1" max="1" width="15.1272727272727" customWidth="1"/>
+    <col min="2" max="2" width="16.1090909090909" customWidth="1"/>
+    <col min="3" max="3" width="18.2090909090909" customWidth="1"/>
+    <col min="4" max="4" width="21.4454545454545" customWidth="1"/>
+    <col min="5" max="5" width="17.1090909090909" customWidth="1"/>
+    <col min="6" max="8" width="53.3363636363636" customWidth="1"/>
+    <col min="9" max="9" width="8.88181818181818" customWidth="1"/>
+    <col min="10" max="10" width="27.3363636363636" customWidth="1"/>
+    <col min="11" max="11" width="40.7545454545455" customWidth="1"/>
+    <col min="12" max="12" width="27.3363636363636" customWidth="1"/>
+    <col min="13" max="13" width="9.33636363636364" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:13">
@@ -1725,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" s="4" customFormat="1" ht="15.15" spans="1:13">
+    <row r="10" s="4" customFormat="1" ht="14.75" spans="1:13">
       <c r="A10" s="10" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Bugfix: Set default value
</commit_message>
<xml_diff>
--- a/resource/excel/Scene.xlsx
+++ b/resource/excel/Scene.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\squick\resource\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A49E766-7FCA-4B43-942C-BD6A035BE815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19095" windowHeight="12585"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -130,14 +136,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -145,158 +145,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,194 +164,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -633,251 +302,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -931,61 +358,17 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+  <cellStyles count="1">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1314,34 +697,34 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.0916666666667" customWidth="1"/>
-    <col min="2" max="4" width="16.0916666666667" customWidth="1"/>
-    <col min="5" max="5" width="18.1833333333333" customWidth="1"/>
-    <col min="6" max="6" width="21.45" customWidth="1"/>
-    <col min="7" max="7" width="17.0916666666667" customWidth="1"/>
-    <col min="8" max="10" width="53.3666666666667" customWidth="1"/>
-    <col min="11" max="11" width="8.90833333333333" customWidth="1"/>
-    <col min="12" max="12" width="27.3666666666667" customWidth="1"/>
-    <col min="13" max="13" width="40.725" customWidth="1"/>
-    <col min="14" max="14" width="27.3666666666667" customWidth="1"/>
-    <col min="15" max="15" width="9.36666666666667" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" customWidth="1"/>
+    <col min="2" max="4" width="16.08984375" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" customWidth="1"/>
+    <col min="8" max="10" width="53.36328125" customWidth="1"/>
+    <col min="11" max="11" width="8.90625" customWidth="1"/>
+    <col min="12" max="12" width="27.36328125" customWidth="1"/>
+    <col min="13" max="13" width="40.7265625" customWidth="1"/>
+    <col min="14" max="14" width="27.36328125" customWidth="1"/>
+    <col min="15" max="15" width="9.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:15">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1388,7 +771,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:15">
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1435,7 +818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="3" customFormat="1" ht="15.75" spans="1:15">
+    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
@@ -1474,12 +857,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="14">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14">
+        <v>0</v>
+      </c>
       <c r="D4" s="14" t="s">
         <v>27</v>
       </c>
@@ -1515,9 +902,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>31</v>
+      </c>
+      <c r="B5" s="14">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -1554,9 +947,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>34</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
@@ -1593,126 +992,126 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="L12" s="13"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="L13" s="13"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="L20" s="13"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="L22" s="13"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="L23" s="13"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
@@ -1720,7 +1119,8 @@
       <c r="L24" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>